<commit_message>
MCQ cleaning integrated into DataAnalysisGUI file. Currently working
</commit_message>
<xml_diff>
--- a/survey_responses_mod_realistic.xlsx
+++ b/survey_responses_mod_realistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEon\Documents\GitHub\Data-Analysis-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB64DD66-BEFD-40FF-A6C1-C36F34096BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D63295-551B-48BF-8CB5-B11509845BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="239">
   <si>
     <t>Gender</t>
   </si>
@@ -136,15 +136,6 @@
     <t>internal survey time calculation</t>
   </si>
   <si>
-    <t xml:space="preserve">MCQ </t>
-  </si>
-  <si>
-    <t>Open-ended</t>
-  </si>
-  <si>
-    <t>No sale in current telco</t>
-  </si>
-  <si>
     <t>Slow and incompetent support staff</t>
   </si>
   <si>
@@ -740,6 +731,12 @@
   </si>
   <si>
     <t>Stop slacking in your job</t>
+  </si>
+  <si>
+    <t>multiple choice</t>
+  </si>
+  <si>
+    <t>open ended</t>
   </si>
 </sst>
 </file>
@@ -1190,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L202" sqref="L202"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1245,7 +1242,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
@@ -1256,34 +1253,34 @@
         <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>39</v>
+        <v>238</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>39</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
@@ -1291,37 +1288,7 @@
         <v>36</v>
       </c>
       <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>1985</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
@@ -1356,7 +1323,7 @@
         <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
@@ -1388,10 +1355,10 @@
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
@@ -1423,10 +1390,10 @@
         <v>21</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
@@ -1458,10 +1425,10 @@
         <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
@@ -1493,10 +1460,10 @@
         <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
@@ -1563,10 +1530,10 @@
         <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
@@ -1598,7 +1565,7 @@
         <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L11" t="s">
         <v>28</v>
@@ -1633,10 +1600,10 @@
         <v>19</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
@@ -1668,10 +1635,10 @@
         <v>20</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
@@ -1706,7 +1673,7 @@
         <v>25</v>
       </c>
       <c r="L14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
@@ -1738,10 +1705,10 @@
         <v>20</v>
       </c>
       <c r="K15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
@@ -1773,10 +1740,10 @@
         <v>21</v>
       </c>
       <c r="K16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.4">
@@ -1811,7 +1778,7 @@
         <v>23</v>
       </c>
       <c r="L17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.4">
@@ -1878,10 +1845,10 @@
         <v>21</v>
       </c>
       <c r="K19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.4">
@@ -1913,10 +1880,10 @@
         <v>20</v>
       </c>
       <c r="K20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.4">
@@ -1948,10 +1915,10 @@
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.4">
@@ -1983,10 +1950,10 @@
         <v>19</v>
       </c>
       <c r="K22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.4">
@@ -2018,7 +1985,7 @@
         <v>20</v>
       </c>
       <c r="K23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L23" t="s">
         <v>30</v>
@@ -2053,10 +2020,10 @@
         <v>21</v>
       </c>
       <c r="K24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.4">
@@ -2088,10 +2055,10 @@
         <v>21</v>
       </c>
       <c r="K25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.4">
@@ -2123,7 +2090,7 @@
         <v>20</v>
       </c>
       <c r="K26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L26" t="s">
         <v>29</v>
@@ -2158,10 +2125,10 @@
         <v>20</v>
       </c>
       <c r="K27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.4">
@@ -2193,10 +2160,10 @@
         <v>19</v>
       </c>
       <c r="K28" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L28" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.4">
@@ -2298,7 +2265,7 @@
         <v>19</v>
       </c>
       <c r="K31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L31" t="s">
         <v>32</v>
@@ -2333,7 +2300,7 @@
         <v>19</v>
       </c>
       <c r="K32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L32" t="s">
         <v>28</v>
@@ -2368,7 +2335,7 @@
         <v>21</v>
       </c>
       <c r="K33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L33" t="s">
         <v>30</v>
@@ -2438,10 +2405,10 @@
         <v>20</v>
       </c>
       <c r="K35" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L35" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.4">
@@ -2476,7 +2443,7 @@
         <v>22</v>
       </c>
       <c r="L36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.4">
@@ -2543,10 +2510,10 @@
         <v>20</v>
       </c>
       <c r="K38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.4">
@@ -2578,10 +2545,10 @@
         <v>21</v>
       </c>
       <c r="K39" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.4">
@@ -2613,7 +2580,7 @@
         <v>20</v>
       </c>
       <c r="K40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L40" t="s">
         <v>29</v>
@@ -2648,10 +2615,10 @@
         <v>19</v>
       </c>
       <c r="K41" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L41" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.4">
@@ -2718,10 +2685,10 @@
         <v>21</v>
       </c>
       <c r="K43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.4">
@@ -2753,7 +2720,7 @@
         <v>20</v>
       </c>
       <c r="K44" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L44" t="s">
         <v>28</v>
@@ -2788,7 +2755,7 @@
         <v>19</v>
       </c>
       <c r="K45" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L45" t="s">
         <v>29</v>
@@ -2826,7 +2793,7 @@
         <v>26</v>
       </c>
       <c r="L46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.4">
@@ -2858,10 +2825,10 @@
         <v>21</v>
       </c>
       <c r="K47" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L47" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.4">
@@ -2963,10 +2930,10 @@
         <v>20</v>
       </c>
       <c r="K50" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L50" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.4">
@@ -2998,10 +2965,10 @@
         <v>21</v>
       </c>
       <c r="K51" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="L51" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.4">
@@ -3106,7 +3073,7 @@
         <v>27</v>
       </c>
       <c r="L54" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.4">
@@ -3138,10 +3105,10 @@
         <v>20</v>
       </c>
       <c r="K55" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L55" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.4">
@@ -3173,10 +3140,10 @@
         <v>20</v>
       </c>
       <c r="K56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.4">
@@ -3208,7 +3175,7 @@
         <v>21</v>
       </c>
       <c r="K57" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L57" t="s">
         <v>32</v>
@@ -3243,10 +3210,10 @@
         <v>20</v>
       </c>
       <c r="K58" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L58" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.4">
@@ -3383,10 +3350,10 @@
         <v>20</v>
       </c>
       <c r="K62" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L62" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.4">
@@ -3453,7 +3420,7 @@
         <v>20</v>
       </c>
       <c r="K64" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L64" t="s">
         <v>30</v>
@@ -3488,10 +3455,10 @@
         <v>19</v>
       </c>
       <c r="K65" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L65" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.4">
@@ -3523,10 +3490,10 @@
         <v>21</v>
       </c>
       <c r="K66" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L66" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.4">
@@ -3558,10 +3525,10 @@
         <v>21</v>
       </c>
       <c r="K67" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L67" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.4">
@@ -3663,10 +3630,10 @@
         <v>19</v>
       </c>
       <c r="K70" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L70" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.4">
@@ -3733,10 +3700,10 @@
         <v>19</v>
       </c>
       <c r="K72" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.4">
@@ -3768,10 +3735,10 @@
         <v>20</v>
       </c>
       <c r="K73" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L73" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.4">
@@ -3803,10 +3770,10 @@
         <v>19</v>
       </c>
       <c r="K74" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L74" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.4">
@@ -3873,10 +3840,10 @@
         <v>20</v>
       </c>
       <c r="K76" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L76" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.4">
@@ -3943,10 +3910,10 @@
         <v>21</v>
       </c>
       <c r="K78" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L78" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.4">
@@ -3978,10 +3945,10 @@
         <v>21</v>
       </c>
       <c r="K79" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L79" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.4">
@@ -4083,10 +4050,10 @@
         <v>19</v>
       </c>
       <c r="K82" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L82" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.4">
@@ -4118,10 +4085,10 @@
         <v>20</v>
       </c>
       <c r="K83" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L83" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.4">
@@ -4153,7 +4120,7 @@
         <v>20</v>
       </c>
       <c r="K84" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L84" t="s">
         <v>29</v>
@@ -4188,10 +4155,10 @@
         <v>20</v>
       </c>
       <c r="K85" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L85" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.4">
@@ -4258,10 +4225,10 @@
         <v>21</v>
       </c>
       <c r="K87" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L87" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.4">
@@ -4293,10 +4260,10 @@
         <v>21</v>
       </c>
       <c r="K88" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="L88" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.4">
@@ -4363,10 +4330,10 @@
         <v>20</v>
       </c>
       <c r="K90" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L90" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.4">
@@ -4468,10 +4435,10 @@
         <v>21</v>
       </c>
       <c r="K93" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L93" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.4">
@@ -4503,10 +4470,10 @@
         <v>21</v>
       </c>
       <c r="K94" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L94" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.4">
@@ -4538,10 +4505,10 @@
         <v>19</v>
       </c>
       <c r="K95" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L95" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.4">
@@ -4643,7 +4610,7 @@
         <v>21</v>
       </c>
       <c r="K98" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L98" t="s">
         <v>28</v>
@@ -4678,10 +4645,10 @@
         <v>20</v>
       </c>
       <c r="K99" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L99" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.4">
@@ -4783,10 +4750,10 @@
         <v>20</v>
       </c>
       <c r="K102" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L102" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.4">
@@ -4818,10 +4785,10 @@
         <v>21</v>
       </c>
       <c r="K103" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="L103" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.4">
@@ -4853,10 +4820,10 @@
         <v>19</v>
       </c>
       <c r="K104" t="s">
+        <v>122</v>
+      </c>
+      <c r="L104" t="s">
         <v>125</v>
-      </c>
-      <c r="L104" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.4">
@@ -4888,10 +4855,10 @@
         <v>20</v>
       </c>
       <c r="K105" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L105" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.4">
@@ -4923,10 +4890,10 @@
         <v>19</v>
       </c>
       <c r="K106" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L106" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.4">
@@ -4958,10 +4925,10 @@
         <v>20</v>
       </c>
       <c r="K107" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L107" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.4">
@@ -5098,10 +5065,10 @@
         <v>19</v>
       </c>
       <c r="K111" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L111" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="112" spans="2:12" x14ac:dyDescent="0.4">
@@ -5133,10 +5100,10 @@
         <v>21</v>
       </c>
       <c r="K112" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L112" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="2:12" x14ac:dyDescent="0.4">
@@ -5168,7 +5135,7 @@
         <v>20</v>
       </c>
       <c r="K113" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L113" t="s">
         <v>28</v>
@@ -5238,10 +5205,10 @@
         <v>19</v>
       </c>
       <c r="K115" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L115" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="116" spans="2:12" x14ac:dyDescent="0.4">
@@ -5273,10 +5240,10 @@
         <v>21</v>
       </c>
       <c r="K116" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L116" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="117" spans="2:12" x14ac:dyDescent="0.4">
@@ -5308,10 +5275,10 @@
         <v>20</v>
       </c>
       <c r="K117" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L117" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="118" spans="2:12" x14ac:dyDescent="0.4">
@@ -5343,10 +5310,10 @@
         <v>20</v>
       </c>
       <c r="K118" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L118" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="119" spans="2:12" x14ac:dyDescent="0.4">
@@ -5378,10 +5345,10 @@
         <v>21</v>
       </c>
       <c r="K119" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L119" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="120" spans="2:12" x14ac:dyDescent="0.4">
@@ -5553,10 +5520,10 @@
         <v>19</v>
       </c>
       <c r="K124" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L124" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="125" spans="2:12" x14ac:dyDescent="0.4">
@@ -5658,10 +5625,10 @@
         <v>21</v>
       </c>
       <c r="K127" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L127" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="128" spans="2:12" x14ac:dyDescent="0.4">
@@ -5693,10 +5660,10 @@
         <v>21</v>
       </c>
       <c r="K128" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L128" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="129" spans="2:12" x14ac:dyDescent="0.4">
@@ -5728,10 +5695,10 @@
         <v>19</v>
       </c>
       <c r="K129" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L129" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="130" spans="2:12" x14ac:dyDescent="0.4">
@@ -5833,10 +5800,10 @@
         <v>19</v>
       </c>
       <c r="K132" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L132" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="133" spans="2:12" x14ac:dyDescent="0.4">
@@ -5903,10 +5870,10 @@
         <v>21</v>
       </c>
       <c r="K134" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L134" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="135" spans="2:12" x14ac:dyDescent="0.4">
@@ -5938,10 +5905,10 @@
         <v>19</v>
       </c>
       <c r="K135" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L135" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="136" spans="2:12" x14ac:dyDescent="0.4">
@@ -5973,10 +5940,10 @@
         <v>21</v>
       </c>
       <c r="K136" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L136" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="137" spans="2:12" x14ac:dyDescent="0.4">
@@ -6043,7 +6010,7 @@
         <v>21</v>
       </c>
       <c r="K138" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L138" t="s">
         <v>30</v>
@@ -6078,7 +6045,7 @@
         <v>20</v>
       </c>
       <c r="K139" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L139" t="s">
         <v>31</v>
@@ -6113,10 +6080,10 @@
         <v>19</v>
       </c>
       <c r="K140" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L140" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="2:12" x14ac:dyDescent="0.4">
@@ -6183,10 +6150,10 @@
         <v>19</v>
       </c>
       <c r="K142" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L142" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="2:12" x14ac:dyDescent="0.4">
@@ -6218,10 +6185,10 @@
         <v>19</v>
       </c>
       <c r="K143" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L143" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="144" spans="2:12" x14ac:dyDescent="0.4">
@@ -6253,10 +6220,10 @@
         <v>19</v>
       </c>
       <c r="K144" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L144" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.4">
@@ -6393,10 +6360,10 @@
         <v>19</v>
       </c>
       <c r="K148" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L148" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.4">
@@ -6431,7 +6398,7 @@
         <v>24</v>
       </c>
       <c r="L149" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.4">
@@ -6498,10 +6465,10 @@
         <v>19</v>
       </c>
       <c r="K151" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L151" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.4">
@@ -6533,10 +6500,10 @@
         <v>20</v>
       </c>
       <c r="K152" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="L152" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.4">
@@ -6673,10 +6640,10 @@
         <v>20</v>
       </c>
       <c r="K156" t="s">
+        <v>172</v>
+      </c>
+      <c r="L156" t="s">
         <v>175</v>
-      </c>
-      <c r="L156" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.4">
@@ -6708,10 +6675,10 @@
         <v>21</v>
       </c>
       <c r="K157" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L157" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.4">
@@ -6746,7 +6713,7 @@
         <v>27</v>
       </c>
       <c r="L158" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.4">
@@ -6778,10 +6745,10 @@
         <v>20</v>
       </c>
       <c r="K159" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L159" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.4">
@@ -6813,10 +6780,10 @@
         <v>21</v>
       </c>
       <c r="K160" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L160" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.4">
@@ -6883,10 +6850,10 @@
         <v>20</v>
       </c>
       <c r="K162" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L162" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.4">
@@ -6918,10 +6885,10 @@
         <v>21</v>
       </c>
       <c r="K163" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L163" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.4">
@@ -6953,10 +6920,10 @@
         <v>19</v>
       </c>
       <c r="K164" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L164" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.4">
@@ -7128,10 +7095,10 @@
         <v>20</v>
       </c>
       <c r="K169" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L169" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="170" spans="2:12" x14ac:dyDescent="0.4">
@@ -7198,10 +7165,10 @@
         <v>19</v>
       </c>
       <c r="K171" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L171" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="172" spans="2:12" x14ac:dyDescent="0.4">
@@ -7233,7 +7200,7 @@
         <v>19</v>
       </c>
       <c r="K172" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L172" t="s">
         <v>29</v>
@@ -7338,10 +7305,10 @@
         <v>19</v>
       </c>
       <c r="K175" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L175" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="176" spans="2:12" x14ac:dyDescent="0.4">
@@ -7373,10 +7340,10 @@
         <v>21</v>
       </c>
       <c r="K176" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L176" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="177" spans="2:12" x14ac:dyDescent="0.4">
@@ -7443,10 +7410,10 @@
         <v>19</v>
       </c>
       <c r="K178" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L178" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="179" spans="2:12" x14ac:dyDescent="0.4">
@@ -7478,10 +7445,10 @@
         <v>20</v>
       </c>
       <c r="K179" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L179" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="180" spans="2:12" x14ac:dyDescent="0.4">
@@ -7513,10 +7480,10 @@
         <v>21</v>
       </c>
       <c r="K180" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L180" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="181" spans="2:12" x14ac:dyDescent="0.4">
@@ -7548,10 +7515,10 @@
         <v>21</v>
       </c>
       <c r="K181" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L181" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="182" spans="2:12" x14ac:dyDescent="0.4">
@@ -7583,10 +7550,10 @@
         <v>20</v>
       </c>
       <c r="K182" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L182" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="183" spans="2:12" x14ac:dyDescent="0.4">
@@ -7618,7 +7585,7 @@
         <v>21</v>
       </c>
       <c r="K183" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L183" t="s">
         <v>31</v>
@@ -7688,10 +7655,10 @@
         <v>21</v>
       </c>
       <c r="K185" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="L185" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="186" spans="2:12" x14ac:dyDescent="0.4">
@@ -7723,10 +7690,10 @@
         <v>20</v>
       </c>
       <c r="K186" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L186" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="187" spans="2:12" x14ac:dyDescent="0.4">
@@ -7758,10 +7725,10 @@
         <v>20</v>
       </c>
       <c r="K187" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L187" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="188" spans="2:12" x14ac:dyDescent="0.4">
@@ -7828,10 +7795,10 @@
         <v>21</v>
       </c>
       <c r="K189" t="s">
+        <v>208</v>
+      </c>
+      <c r="L189" t="s">
         <v>211</v>
-      </c>
-      <c r="L189" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="190" spans="2:12" x14ac:dyDescent="0.4">
@@ -7863,10 +7830,10 @@
         <v>21</v>
       </c>
       <c r="K190" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L190" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="191" spans="2:12" x14ac:dyDescent="0.4">
@@ -7898,10 +7865,10 @@
         <v>19</v>
       </c>
       <c r="K191" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L191" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="192" spans="2:12" x14ac:dyDescent="0.4">
@@ -7933,10 +7900,10 @@
         <v>20</v>
       </c>
       <c r="K192" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L192" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="193" spans="2:12" x14ac:dyDescent="0.4">
@@ -7968,10 +7935,10 @@
         <v>21</v>
       </c>
       <c r="K193" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L193" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="194" spans="2:12" x14ac:dyDescent="0.4">
@@ -8006,7 +7973,7 @@
         <v>24</v>
       </c>
       <c r="L194" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="195" spans="2:12" x14ac:dyDescent="0.4">
@@ -8108,10 +8075,10 @@
         <v>19</v>
       </c>
       <c r="K197" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L197" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="198" spans="2:12" x14ac:dyDescent="0.4">
@@ -8181,7 +8148,7 @@
         <v>24</v>
       </c>
       <c r="L199" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="200" spans="2:12" x14ac:dyDescent="0.4">
@@ -8213,10 +8180,10 @@
         <v>19</v>
       </c>
       <c r="K200" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L200" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="201" spans="2:12" x14ac:dyDescent="0.4">
@@ -8248,10 +8215,10 @@
         <v>21</v>
       </c>
       <c r="K201" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L201" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="202" spans="2:12" x14ac:dyDescent="0.4">
@@ -8263,6 +8230,30 @@
       </c>
       <c r="D202">
         <v>1987</v>
+      </c>
+      <c r="E202" t="s">
+        <v>11</v>
+      </c>
+      <c r="F202" t="s">
+        <v>17</v>
+      </c>
+      <c r="G202">
+        <v>1</v>
+      </c>
+      <c r="H202">
+        <v>2</v>
+      </c>
+      <c r="I202">
+        <v>5</v>
+      </c>
+      <c r="J202" t="s">
+        <v>21</v>
+      </c>
+      <c r="K202" t="s">
+        <v>222</v>
+      </c>
+      <c r="L202" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a function to open a temporary excel file
</commit_message>
<xml_diff>
--- a/survey_responses_mod_realistic.xlsx
+++ b/survey_responses_mod_realistic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SIT\Trimester 1\INF 1002\Project\Data-Analysis-Project-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEon\Documents\GitHub\Data-Analysis-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D66743-111A-48CA-8C04-613B4D3AC97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77780062-307C-41CC-BF0C-68F5D76A4646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="239">
   <si>
     <t>Gender</t>
   </si>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L209" sqref="L209"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1334,9 +1334,6 @@
       <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
       <c r="L3" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
updated realistic excel file
</commit_message>
<xml_diff>
--- a/survey_responses_mod_realistic.xlsx
+++ b/survey_responses_mod_realistic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEon\Documents\GitHub\Data-Analysis-Project-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\Data-Analysis-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77780062-307C-41CC-BF0C-68F5D76A4646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1F1943-D9D9-4BDE-8A3A-2430666C7F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="240">
   <si>
     <t>Gender</t>
   </si>
@@ -737,6 +737,9 @@
   </si>
   <si>
     <t>open ended</t>
+  </si>
+  <si>
+    <t>Cheaper from if get from others</t>
   </si>
 </sst>
 </file>
@@ -1207,27 +1210,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.69140625" customWidth="1"/>
-    <col min="2" max="2" width="17.23046875" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="16.69140625" customWidth="1"/>
-    <col min="6" max="6" width="17.3046875" customWidth="1"/>
-    <col min="7" max="7" width="17.765625" customWidth="1"/>
-    <col min="8" max="8" width="18.23046875" customWidth="1"/>
-    <col min="9" max="9" width="21.3046875" customWidth="1"/>
-    <col min="10" max="10" width="22.84375" customWidth="1"/>
-    <col min="11" max="11" width="42.07421875" customWidth="1"/>
-    <col min="12" max="12" width="45.4609375" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" customWidth="1"/>
+    <col min="9" max="9" width="21.26953125" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" customWidth="1"/>
+    <col min="11" max="11" width="42.08984375" customWidth="1"/>
+    <col min="12" max="12" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="31.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
@@ -1303,7 +1306,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
@@ -1316,29 +1319,14 @@
       <c r="D3">
         <v>1979</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
+      <c r="K3" t="s">
+        <v>239</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>16</v>
       </c>
@@ -1373,7 +1361,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>20</v>
       </c>
@@ -1408,7 +1396,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>4</v>
       </c>
@@ -1443,7 +1431,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>7</v>
       </c>
@@ -1478,7 +1466,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>18</v>
       </c>
@@ -1513,7 +1501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>15</v>
       </c>
@@ -1548,7 +1536,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>18</v>
       </c>
@@ -1583,7 +1571,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>12</v>
       </c>
@@ -1618,7 +1606,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>16</v>
       </c>
@@ -1653,7 +1641,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>18</v>
       </c>
@@ -1688,7 +1676,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>7</v>
       </c>
@@ -1723,7 +1711,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>6</v>
       </c>
@@ -1758,7 +1746,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>6</v>
       </c>
@@ -1793,7 +1781,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>4</v>
       </c>
@@ -1828,7 +1816,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>17</v>
       </c>
@@ -1863,7 +1851,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>20</v>
       </c>
@@ -1898,7 +1886,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>4</v>
       </c>
@@ -1933,7 +1921,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>20</v>
       </c>
@@ -1968,7 +1956,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>10</v>
       </c>
@@ -2003,7 +1991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>3</v>
       </c>
@@ -2038,7 +2026,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>4</v>
       </c>
@@ -2073,7 +2061,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>9</v>
       </c>
@@ -2108,7 +2096,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>18</v>
       </c>
@@ -2143,7 +2131,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>15</v>
       </c>
@@ -2178,7 +2166,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>11</v>
       </c>
@@ -2213,7 +2201,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>16</v>
       </c>
@@ -2248,7 +2236,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>8</v>
       </c>
@@ -2283,7 +2271,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>4</v>
       </c>
@@ -2318,7 +2306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>6</v>
       </c>
@@ -2353,7 +2341,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>3</v>
       </c>
@@ -2388,7 +2376,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>19</v>
       </c>
@@ -2423,7 +2411,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>6</v>
       </c>
@@ -2458,7 +2446,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>8</v>
       </c>
@@ -2493,7 +2481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>15</v>
       </c>
@@ -2528,7 +2516,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>20</v>
       </c>
@@ -2563,7 +2551,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>11</v>
       </c>
@@ -2598,7 +2586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>7</v>
       </c>
@@ -2633,7 +2621,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>3</v>
       </c>
@@ -2668,7 +2656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>20</v>
       </c>
@@ -2703,7 +2691,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>4</v>
       </c>
@@ -2738,7 +2726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>4</v>
       </c>
@@ -2773,7 +2761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>9</v>
       </c>
@@ -2808,7 +2796,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>3</v>
       </c>
@@ -2843,7 +2831,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>12</v>
       </c>
@@ -2878,7 +2866,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>7</v>
       </c>
@@ -2913,7 +2901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>9</v>
       </c>
@@ -2948,7 +2936,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B50">
         <v>8</v>
       </c>
@@ -2983,7 +2971,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B51">
         <v>12</v>
       </c>
@@ -3018,7 +3006,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B52">
         <v>14</v>
       </c>
@@ -3053,7 +3041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53">
         <v>10</v>
       </c>
@@ -3088,7 +3076,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B54">
         <v>3</v>
       </c>
@@ -3123,7 +3111,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B55">
         <v>5</v>
       </c>
@@ -3158,7 +3146,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B56">
         <v>19</v>
       </c>
@@ -3193,7 +3181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B57">
         <v>4</v>
       </c>
@@ -3228,7 +3216,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B58">
         <v>18</v>
       </c>
@@ -3263,7 +3251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B59">
         <v>11</v>
       </c>
@@ -3298,7 +3286,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B60">
         <v>13</v>
       </c>
@@ -3333,7 +3321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B61">
         <v>16</v>
       </c>
@@ -3368,7 +3356,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B62">
         <v>6</v>
       </c>
@@ -3403,7 +3391,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B63">
         <v>6</v>
       </c>
@@ -3438,7 +3426,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B64">
         <v>4</v>
       </c>
@@ -3473,7 +3461,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B65">
         <v>3</v>
       </c>
@@ -3508,7 +3496,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B66">
         <v>11</v>
       </c>
@@ -3543,7 +3531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B67">
         <v>4</v>
       </c>
@@ -3578,7 +3566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B68">
         <v>9</v>
       </c>
@@ -3613,7 +3601,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B69">
         <v>4</v>
       </c>
@@ -3648,7 +3636,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B70">
         <v>16</v>
       </c>
@@ -3683,7 +3671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B71">
         <v>7</v>
       </c>
@@ -3718,7 +3706,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B72">
         <v>3</v>
       </c>
@@ -3753,7 +3741,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B73">
         <v>16</v>
       </c>
@@ -3788,7 +3776,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B74">
         <v>11</v>
       </c>
@@ -3823,7 +3811,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B75">
         <v>18</v>
       </c>
@@ -3858,7 +3846,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B76">
         <v>9</v>
       </c>
@@ -3893,7 +3881,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B77">
         <v>5</v>
       </c>
@@ -3928,7 +3916,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B78">
         <v>20</v>
       </c>
@@ -3963,7 +3951,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B79">
         <v>8</v>
       </c>
@@ -3998,7 +3986,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B80">
         <v>17</v>
       </c>
@@ -4033,7 +4021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B81">
         <v>3</v>
       </c>
@@ -4068,7 +4056,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B82">
         <v>14</v>
       </c>
@@ -4103,7 +4091,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B83">
         <v>7</v>
       </c>
@@ -4138,7 +4126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B84">
         <v>6</v>
       </c>
@@ -4173,7 +4161,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B85">
         <v>17</v>
       </c>
@@ -4208,7 +4196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B86">
         <v>5</v>
       </c>
@@ -4243,7 +4231,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B87">
         <v>18</v>
       </c>
@@ -4278,7 +4266,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B88">
         <v>3</v>
       </c>
@@ -4313,7 +4301,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B89">
         <v>16</v>
       </c>
@@ -4348,7 +4336,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B90">
         <v>10</v>
       </c>
@@ -4383,7 +4371,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B91">
         <v>19</v>
       </c>
@@ -4418,7 +4406,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="92" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B92">
         <v>6</v>
       </c>
@@ -4453,7 +4441,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B93">
         <v>3</v>
       </c>
@@ -4488,7 +4476,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B94">
         <v>15</v>
       </c>
@@ -4523,7 +4511,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="95" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B95">
         <v>20</v>
       </c>
@@ -4558,7 +4546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B96">
         <v>17</v>
       </c>
@@ -4593,7 +4581,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B97">
         <v>11</v>
       </c>
@@ -4628,7 +4616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="98" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B98">
         <v>14</v>
       </c>
@@ -4663,7 +4651,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="99" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B99">
         <v>4</v>
       </c>
@@ -4698,7 +4686,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="100" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B100">
         <v>7</v>
       </c>
@@ -4733,7 +4721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B101">
         <v>13</v>
       </c>
@@ -4768,7 +4756,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="102" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B102">
         <v>9</v>
       </c>
@@ -4803,7 +4791,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="103" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B103">
         <v>13</v>
       </c>
@@ -4838,7 +4826,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="104" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B104">
         <v>3</v>
       </c>
@@ -4873,7 +4861,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="105" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B105">
         <v>6</v>
       </c>
@@ -4908,7 +4896,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="106" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B106">
         <v>10</v>
       </c>
@@ -4943,7 +4931,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B107">
         <v>7</v>
       </c>
@@ -4978,7 +4966,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="108" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B108">
         <v>5</v>
       </c>
@@ -5013,7 +5001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="109" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B109">
         <v>7</v>
       </c>
@@ -5048,7 +5036,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="110" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B110">
         <v>9</v>
       </c>
@@ -5083,7 +5071,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="111" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B111">
         <v>14</v>
       </c>
@@ -5118,7 +5106,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="112" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B112">
         <v>18</v>
       </c>
@@ -5153,7 +5141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="113" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B113">
         <v>9</v>
       </c>
@@ -5188,7 +5176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="114" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B114">
         <v>16</v>
       </c>
@@ -5223,7 +5211,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="115" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B115">
         <v>4</v>
       </c>
@@ -5258,7 +5246,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="116" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="116" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B116">
         <v>3</v>
       </c>
@@ -5293,7 +5281,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="117" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B117">
         <v>9</v>
       </c>
@@ -5328,7 +5316,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="118" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="118" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B118">
         <v>5</v>
       </c>
@@ -5363,7 +5351,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="119" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="119" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B119">
         <v>19</v>
       </c>
@@ -5398,7 +5386,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="120" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="120" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B120">
         <v>15</v>
       </c>
@@ -5433,7 +5421,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="121" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B121">
         <v>12</v>
       </c>
@@ -5468,7 +5456,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B122">
         <v>8</v>
       </c>
@@ -5503,7 +5491,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="123" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B123">
         <v>10</v>
       </c>
@@ -5538,7 +5526,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="124" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="124" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B124">
         <v>20</v>
       </c>
@@ -5573,7 +5561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="125" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="125" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B125">
         <v>7</v>
       </c>
@@ -5608,7 +5596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="126" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B126">
         <v>20</v>
       </c>
@@ -5643,7 +5631,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="127" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="127" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B127">
         <v>3</v>
       </c>
@@ -5678,7 +5666,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="128" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B128">
         <v>10</v>
       </c>
@@ -5713,7 +5701,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="129" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B129">
         <v>4</v>
       </c>
@@ -5748,7 +5736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="130" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B130">
         <v>8</v>
       </c>
@@ -5783,7 +5771,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="131" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="131" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B131">
         <v>8</v>
       </c>
@@ -5818,7 +5806,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="132" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="132" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B132">
         <v>4</v>
       </c>
@@ -5853,7 +5841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="133" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B133">
         <v>16</v>
       </c>
@@ -5888,7 +5876,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="134" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="134" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B134">
         <v>9</v>
       </c>
@@ -5923,7 +5911,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="135" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="135" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B135">
         <v>6</v>
       </c>
@@ -5958,7 +5946,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="136" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="136" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B136">
         <v>13</v>
       </c>
@@ -5993,7 +5981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="137" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="137" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B137">
         <v>5</v>
       </c>
@@ -6028,7 +6016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="138" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="138" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B138">
         <v>5</v>
       </c>
@@ -6063,7 +6051,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="139" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="139" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B139">
         <v>4</v>
       </c>
@@ -6098,7 +6086,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="140" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="140" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B140">
         <v>15</v>
       </c>
@@ -6133,7 +6121,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="141" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B141">
         <v>16</v>
       </c>
@@ -6168,7 +6156,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="142" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="142" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B142">
         <v>11</v>
       </c>
@@ -6203,7 +6191,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="143" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="143" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B143">
         <v>8</v>
       </c>
@@ -6238,7 +6226,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="144" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B144">
         <v>4</v>
       </c>
@@ -6273,7 +6261,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B145">
         <v>3</v>
       </c>
@@ -6308,7 +6296,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B146">
         <v>11</v>
       </c>
@@ -6343,7 +6331,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B147">
         <v>5</v>
       </c>
@@ -6378,7 +6366,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="148" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B148">
         <v>20</v>
       </c>
@@ -6413,7 +6401,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="149" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B149">
         <v>11</v>
       </c>
@@ -6448,7 +6436,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B150">
         <v>3</v>
       </c>
@@ -6483,7 +6471,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="151" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B151">
         <v>4</v>
       </c>
@@ -6518,7 +6506,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="152" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B152">
         <v>13</v>
       </c>
@@ -6553,7 +6541,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B153">
         <v>12</v>
       </c>
@@ -6588,7 +6576,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="154" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B154">
         <v>6</v>
       </c>
@@ -6623,7 +6611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="155" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B155">
         <v>15</v>
       </c>
@@ -6658,7 +6646,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="156" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B156">
         <v>11</v>
       </c>
@@ -6693,7 +6681,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="157" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="157" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B157">
         <v>5</v>
       </c>
@@ -6728,7 +6716,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="158" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="158" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B158">
         <v>3</v>
       </c>
@@ -6763,7 +6751,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="159" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="159" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B159">
         <v>9</v>
       </c>
@@ -6798,7 +6786,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="160" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="160" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B160">
         <v>12</v>
       </c>
@@ -6833,7 +6821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="161" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="161" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B161">
         <v>3</v>
       </c>
@@ -6868,7 +6856,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="162" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B162">
         <v>10</v>
       </c>
@@ -6903,7 +6891,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="163" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="163" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B163">
         <v>9</v>
       </c>
@@ -6938,7 +6926,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="164" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="164" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B164">
         <v>5</v>
       </c>
@@ -6973,7 +6961,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="165" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B165">
         <v>16</v>
       </c>
@@ -7008,7 +6996,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="166" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="166" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B166">
         <v>20</v>
       </c>
@@ -7043,7 +7031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="167" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="167" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B167">
         <v>12</v>
       </c>
@@ -7078,7 +7066,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="168" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B168">
         <v>17</v>
       </c>
@@ -7113,7 +7101,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="169" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="169" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B169">
         <v>15</v>
       </c>
@@ -7148,7 +7136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="170" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B170">
         <v>17</v>
       </c>
@@ -7183,7 +7171,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="171" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B171">
         <v>10</v>
       </c>
@@ -7218,7 +7206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="172" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="172" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B172">
         <v>13</v>
       </c>
@@ -7253,7 +7241,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="173" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="173" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B173">
         <v>13</v>
       </c>
@@ -7288,7 +7276,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="174" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="174" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B174">
         <v>4</v>
       </c>
@@ -7323,7 +7311,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="175" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="175" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B175">
         <v>19</v>
       </c>
@@ -7358,7 +7346,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="176" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="176" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B176">
         <v>14</v>
       </c>
@@ -7393,7 +7381,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B177">
         <v>10</v>
       </c>
@@ -7428,7 +7416,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="178" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="178" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B178">
         <v>16</v>
       </c>
@@ -7463,7 +7451,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="179" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="179" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B179">
         <v>18</v>
       </c>
@@ -7498,7 +7486,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="180" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B180">
         <v>5</v>
       </c>
@@ -7533,7 +7521,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="181" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="181" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B181">
         <v>7</v>
       </c>
@@ -7568,7 +7556,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="182" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B182">
         <v>6</v>
       </c>
@@ -7603,7 +7591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="183" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="183" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B183">
         <v>11</v>
       </c>
@@ -7638,7 +7626,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="184" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B184">
         <v>14</v>
       </c>
@@ -7673,7 +7661,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="185" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B185">
         <v>11</v>
       </c>
@@ -7708,7 +7696,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="186" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="186" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B186">
         <v>5</v>
       </c>
@@ -7743,7 +7731,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="187" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="187" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B187">
         <v>8</v>
       </c>
@@ -7778,7 +7766,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="188" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="188" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B188">
         <v>4</v>
       </c>
@@ -7813,7 +7801,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="189" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="189" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B189">
         <v>3</v>
       </c>
@@ -7848,7 +7836,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="190" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="190" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B190">
         <v>5</v>
       </c>
@@ -7883,7 +7871,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="191" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="191" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B191">
         <v>5</v>
       </c>
@@ -7918,7 +7906,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="192" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="192" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B192">
         <v>9</v>
       </c>
@@ -7953,7 +7941,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="193" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="193" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B193">
         <v>3</v>
       </c>
@@ -7988,7 +7976,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="194" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="194" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B194">
         <v>4</v>
       </c>
@@ -8023,7 +8011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="195" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B195">
         <v>12</v>
       </c>
@@ -8058,7 +8046,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="196" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="196" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B196">
         <v>14</v>
       </c>
@@ -8093,7 +8081,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="197" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="197" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B197">
         <v>7</v>
       </c>
@@ -8128,7 +8116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="198" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="198" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B198">
         <v>3</v>
       </c>
@@ -8163,7 +8151,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="199" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="199" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B199">
         <v>4</v>
       </c>
@@ -8198,7 +8186,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="200" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="200" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B200">
         <v>8</v>
       </c>
@@ -8233,7 +8221,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="201" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="201" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B201">
         <v>8</v>
       </c>

</xml_diff>